<commit_message>
plot af SiO2 mm
</commit_message>
<xml_diff>
--- a/data/Multi_salt_alle_change_pH.xlsx
+++ b/data/Multi_salt_alle_change_pH.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/992765_grundfos_com/Documents/Code/Speciale/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="8_{B4563AA1-F904-427B-AF4F-96957668340D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{630A58AE-0E28-4B27-8B26-1E73D85D8773}"/>
+  <xr:revisionPtr revIDLastSave="141" documentId="8_{B4563AA1-F904-427B-AF4F-96957668340D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F224B910-3713-4680-8D33-4AACC9C147BD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
+    <workbookView xWindow="-25680" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
   </bookViews>
   <sheets>
     <sheet name="pH 9.2" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <author>Steffen Lykke Christensen</author>
   </authors>
   <commentList>
-    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{326DB34D-FEAC-4F14-AE49-3242A1440A67}">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{326DB34D-FEAC-4F14-AE49-3242A1440A67}">
       <text>
         <r>
           <rPr>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="16">
   <si>
     <t>Na  [mg/l]</t>
   </si>
@@ -234,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -247,9 +247,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -576,491 +573,485 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E6429C-0FFF-4E30-BF3A-6A5B96E649C1}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="8"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="str">
+        <f t="shared" ref="C2:C13" si="0">CONCATENATE("M","-9.2-",A2,"-F")</f>
+        <v>M-9.2-0-F</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6">
+        <v>40.4</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2">
+        <v>1339</v>
+      </c>
+      <c r="K2">
+        <v>9.11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>3.5</v>
+      </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>M-9.2-3,5-F</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6">
+        <v>42.9</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3">
+        <v>1527</v>
+      </c>
+      <c r="K3">
+        <v>9.19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="str">
-        <f t="shared" ref="C4:C15" si="0">CONCATENATE("M","-9.2-",A4,"-F")</f>
-        <v>M-9.2-0-F</v>
+        <f>CONCATENATE("M","-9.2-",A4,"-P")</f>
+        <v>M-9.2-3,5-P</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="6">
-        <v>40.4</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4">
-        <v>1339</v>
+        <v>813</v>
       </c>
       <c r="K4">
-        <v>9.11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+        <v>8.57</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-3,5-F</v>
+        <v>M-9.2-5-F</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="6">
-        <v>42.9</v>
+        <v>42.2</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5">
-        <v>1527</v>
+        <v>1708</v>
       </c>
       <c r="K5">
-        <v>9.19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>9.23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A6,"-P")</f>
-        <v>M-9.2-3,5-P</v>
+        <v>M-9.2-5-P</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="6">
-        <v>33.799999999999997</v>
+        <v>35.5</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6">
-        <v>813</v>
+        <v>882</v>
       </c>
       <c r="K6">
-        <v>8.57</v>
-      </c>
-      <c r="L6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+        <v>8.56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-5-F</v>
+        <v>M-9.2-6-F</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="6">
-        <v>42.2</v>
+        <v>45.3</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7">
-        <v>1708</v>
+        <v>1856</v>
       </c>
       <c r="K7">
-        <v>9.23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A8,"-P")</f>
-        <v>M-9.2-5-P</v>
+        <v>M-9.2-6-P</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="6">
-        <v>35.5</v>
-      </c>
-      <c r="I8" s="6"/>
+        <v>41.3</v>
+      </c>
+      <c r="I8" s="6">
+        <v>36.5</v>
+      </c>
       <c r="J8">
-        <v>882</v>
+        <v>945</v>
       </c>
       <c r="K8">
-        <v>8.56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>8.57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-6-F</v>
+        <v>M-9.2-7-F</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="6">
-        <v>45.3</v>
+        <v>48.4</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9">
-        <v>1856</v>
+        <v>2050</v>
       </c>
       <c r="K9">
-        <v>9.24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>9.2799999999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A10,"-P")</f>
-        <v>M-9.2-6-P</v>
+        <v>M-9.2-7-P</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="6">
-        <v>41.3</v>
-      </c>
-      <c r="I10" s="6">
-        <v>36.5</v>
-      </c>
+        <v>37.299999999999997</v>
+      </c>
+      <c r="I10" s="6"/>
       <c r="J10">
-        <v>945</v>
+        <v>1027</v>
       </c>
       <c r="K10">
-        <v>8.57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+        <v>8.58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-7-F</v>
+        <v>M-9.2-8-F</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="6">
-        <v>48.4</v>
+        <v>50.2</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11">
-        <v>2050</v>
+        <v>2350</v>
       </c>
       <c r="K11">
-        <v>9.2799999999999994</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+        <v>9.32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A12,"-P")</f>
-        <v>M-9.2-7-P</v>
+        <v>M-9.2-8-P</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="6">
-        <v>37.299999999999997</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12">
-        <v>1027</v>
+        <v>1130</v>
       </c>
       <c r="K12">
-        <v>8.58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+        <v>8.59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-8-F</v>
+        <v>M-9.2-9-F</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="6">
-        <v>50.2</v>
+        <v>55.4</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13">
-        <v>2350</v>
+        <v>2710</v>
       </c>
       <c r="K13">
-        <v>9.32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+        <v>9.2899999999999991</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A14,"-P")</f>
-        <v>M-9.2-8-P</v>
+        <v>M-9.2-9-P</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="6">
-        <v>38.299999999999997</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14">
-        <v>1130</v>
+        <v>1133</v>
       </c>
       <c r="K14">
-        <v>8.59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+        <v>8.6300000000000008</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3" t="str">
+        <f>CONCATENATE("Bi-M","-9.2-",A18,"-F")</f>
+        <v>Bi-M-9.2-0-F</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="3" t="str">
+        <f t="shared" ref="C19:C23" si="1">CONCATENATE("Bi-M","-9.2-",A19,"-F")</f>
+        <v>Bi-M-9.2-0-F</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Bi-M-9.2-6-F</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Bi-M-9.2-6-F</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>M-9.2-9-F</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6">
-        <v>55.4</v>
-      </c>
-      <c r="I15" s="6"/>
-      <c r="J15">
-        <v>2710</v>
-      </c>
-      <c r="K15">
-        <v>9.2899999999999991</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>9</v>
-      </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="3" t="str">
-        <f>CONCATENATE("M","-9.2-",A16,"-P")</f>
-        <v>M-9.2-9-P</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6">
-        <v>40.200000000000003</v>
-      </c>
-      <c r="I16" s="6"/>
-      <c r="J16">
-        <v>1133</v>
-      </c>
-      <c r="K16">
-        <v>8.6300000000000008</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>0</v>
-      </c>
-      <c r="B20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="3" t="str">
-        <f>CONCATENATE("Bi-M","-9.2-",A20,"-F")</f>
-        <v>Bi-M-9.2-0-F</v>
-      </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>0</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="3" t="str">
-        <f t="shared" ref="C21:C25" si="1">CONCATENATE("Bi-M","-9.2-",A21,"-F")</f>
-        <v>Bi-M-9.2-0-F</v>
-      </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>6</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>Bi-M-9.2-6-F</v>
+        <v>Bi-M-9.2-9-F</v>
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>Bi-M-9.2-6-F</v>
+        <v>Bi-M-9.2-9-F</v>
       </c>
       <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>9</v>
-      </c>
-      <c r="B24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Bi-M-9.2-9-F</v>
-      </c>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>9</v>
-      </c>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Bi-M-9.2-9-F</v>
-      </c>
-      <c r="D25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1077,17 +1068,17 @@
       <selection activeCell="C4" sqref="C4:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1116,7 +1107,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -1134,7 +1125,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3.5</v>
       </c>
@@ -1152,7 +1143,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3.5</v>
       </c>
@@ -1170,7 +1161,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1188,7 +1179,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1206,7 +1197,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1224,7 +1215,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -1242,7 +1233,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -1260,7 +1251,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7</v>
       </c>
@@ -1278,7 +1269,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -1296,7 +1287,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>8</v>
       </c>
@@ -1314,7 +1305,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>9</v>
       </c>
@@ -1332,7 +1323,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>9</v>
       </c>
@@ -1350,12 +1341,12 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -1368,7 +1359,7 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>0</v>
       </c>
@@ -1381,7 +1372,7 @@
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>6</v>
       </c>
@@ -1394,7 +1385,7 @@
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>6</v>
       </c>
@@ -1407,7 +1398,7 @@
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>9</v>
       </c>
@@ -1420,7 +1411,7 @@
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>9</v>
       </c>
@@ -1447,17 +1438,17 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1486,7 +1477,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -1504,7 +1495,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3.5</v>
       </c>
@@ -1522,7 +1513,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3.5</v>
       </c>
@@ -1540,7 +1531,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1558,7 +1549,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1576,7 +1567,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1594,7 +1585,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -1612,7 +1603,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -1630,7 +1621,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7</v>
       </c>
@@ -1648,7 +1639,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -1666,7 +1657,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>8</v>
       </c>
@@ -1684,7 +1675,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>9</v>
       </c>
@@ -1702,7 +1693,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>9</v>
       </c>
@@ -1720,12 +1711,12 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -1738,7 +1729,7 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>0</v>
       </c>
@@ -1751,7 +1742,7 @@
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>6</v>
       </c>
@@ -1764,7 +1755,7 @@
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>6</v>
       </c>
@@ -1777,7 +1768,7 @@
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>9</v>
       </c>
@@ -1790,7 +1781,7 @@
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
SiO2 multisalt pH 10, og mere data behandling
</commit_message>
<xml_diff>
--- a/data/Multi_salt_alle_change_pH.xlsx
+++ b/data/Multi_salt_alle_change_pH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="8_{B4563AA1-F904-427B-AF4F-96957668340D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F224B910-3713-4680-8D33-4AACC9C147BD}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="8_{B4563AA1-F904-427B-AF4F-96957668340D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{76E28FBB-C54D-48C3-BE39-DFAB772270B9}"/>
   <bookViews>
-    <workbookView xWindow="-25680" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
+    <workbookView xWindow="-25290" yWindow="675" windowWidth="21600" windowHeight="11280" activeTab="1" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
   </bookViews>
   <sheets>
     <sheet name="pH 9.2" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="16">
   <si>
     <t>Na  [mg/l]</t>
   </si>
@@ -575,21 +575,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E6429C-0FFF-4E30-BF3A-6A5B96E649C1}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -627,7 +627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -653,7 +653,7 @@
         <v>9.11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>3.5</v>
       </c>
@@ -679,7 +679,7 @@
         <v>9.19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3.5</v>
       </c>
@@ -708,7 +708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -734,7 +734,7 @@
         <v>9.23</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -760,7 +760,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -786,7 +786,7 @@
         <v>9.24</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -814,7 +814,7 @@
         <v>8.57</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -840,7 +840,7 @@
         <v>9.2799999999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -866,7 +866,7 @@
         <v>8.58</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -892,7 +892,7 @@
         <v>9.32</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -918,7 +918,7 @@
         <v>8.59</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -944,7 +944,7 @@
         <v>9.2899999999999991</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>9</v>
       </c>
@@ -970,12 +970,12 @@
         <v>8.6300000000000008</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -988,7 +988,7 @@
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>0</v>
       </c>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>6</v>
       </c>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>6</v>
       </c>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>9</v>
       </c>
@@ -1040,7 +1040,7 @@
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>9</v>
       </c>
@@ -1062,151 +1062,196 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A17F5B53-D1CD-43A2-82D9-8A2F69E97C05}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="str">
+        <f t="shared" ref="C2:C13" si="0">CONCATENATE("M","-9.2-",A2,"-F")</f>
+        <v>M-9.2-0-F</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1.25</v>
+      </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>M-9.2-1,25-F</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6">
+        <v>44.4</v>
+      </c>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="str">
-        <f t="shared" ref="C4:C15" si="0">CONCATENATE("M","-9.2-",A4,"-F")</f>
-        <v>M-9.2-0-F</v>
+        <f>CONCATENATE("M","-9.2-",A4,"-P")</f>
+        <v>M-9.2-1,25-P</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
+      <c r="H4" s="6">
+        <v>22.4</v>
+      </c>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-3,5-F</v>
+        <v>M-9.2-3-F</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
+      <c r="H5" s="6">
+        <v>48.6</v>
+      </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A6,"-P")</f>
-        <v>M-9.2-3,5-P</v>
+        <v>M-9.2-3-P</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
+      <c r="H6" s="6">
+        <v>25.5</v>
+      </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-5-F</v>
+        <v>M-9.2-4-F</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
+      <c r="H7" s="6">
+        <v>53.5</v>
+      </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A8,"-P")</f>
-        <v>M-9.2-5-P</v>
+        <v>M-9.2-4-P</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
+      <c r="H8" s="6">
+        <v>25</v>
+      </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-6-F</v>
+        <v>M-9.2-5-F</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1215,16 +1260,16 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A10,"-P")</f>
-        <v>M-9.2-6-P</v>
+        <v>M-9.2-5-P</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1233,16 +1278,16 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-7-F</v>
+        <v>M-9.2-6-F</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1251,16 +1296,16 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A12,"-P")</f>
-        <v>M-9.2-7-P</v>
+        <v>M-9.2-6-P</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1269,16 +1314,16 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-8-F</v>
+        <v>M-9.2-7-F</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1287,16 +1332,16 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A14,"-P")</f>
-        <v>M-9.2-8-P</v>
+        <v>M-9.2-7-P</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1305,124 +1350,88 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3" t="str">
+        <f>CONCATENATE("Bi-M","-9.2-",A18,"-F")</f>
+        <v>Bi-M-9.2-0-F</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="3" t="str">
+        <f t="shared" ref="C19:C23" si="1">CONCATENATE("Bi-M","-9.2-",A19,"-F")</f>
+        <v>Bi-M-9.2-0-F</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Bi-M-9.2-6-F</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Bi-M-9.2-6-F</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>M-9.2-9-F</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>9</v>
-      </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="3" t="str">
-        <f>CONCATENATE("M","-9.2-",A16,"-P")</f>
-        <v>M-9.2-9-P</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>0</v>
-      </c>
-      <c r="B20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="3" t="str">
-        <f>CONCATENATE("Bi-M","-9.2-",A20,"-F")</f>
-        <v>Bi-M-9.2-0-F</v>
-      </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>0</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="3" t="str">
-        <f t="shared" ref="C21:C25" si="1">CONCATENATE("Bi-M","-9.2-",A21,"-F")</f>
-        <v>Bi-M-9.2-0-F</v>
-      </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>6</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>Bi-M-9.2-6-F</v>
+        <v>Bi-M-9.2-9-F</v>
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>Bi-M-9.2-6-F</v>
+        <v>Bi-M-9.2-9-F</v>
       </c>
       <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>9</v>
-      </c>
-      <c r="B24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Bi-M-9.2-9-F</v>
-      </c>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>9</v>
-      </c>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Bi-M-9.2-9-F</v>
-      </c>
-      <c r="D25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1438,17 +1447,17 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1477,7 +1486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -1495,7 +1504,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3.5</v>
       </c>
@@ -1513,7 +1522,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3.5</v>
       </c>
@@ -1531,7 +1540,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1549,7 +1558,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1567,7 +1576,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1585,7 +1594,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -1603,7 +1612,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -1621,7 +1630,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>7</v>
       </c>
@@ -1639,7 +1648,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -1657,7 +1666,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>8</v>
       </c>
@@ -1675,7 +1684,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>9</v>
       </c>
@@ -1693,7 +1702,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>9</v>
       </c>
@@ -1711,12 +1720,12 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -1729,7 +1738,7 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>0</v>
       </c>
@@ -1742,7 +1751,7 @@
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>6</v>
       </c>
@@ -1755,7 +1764,7 @@
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>6</v>
       </c>
@@ -1768,7 +1777,7 @@
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>9</v>
       </c>
@@ -1781,7 +1790,7 @@
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
data behandling for pH 9.2 so far
</commit_message>
<xml_diff>
--- a/data/Multi_salt_alle_change_pH.xlsx
+++ b/data/Multi_salt_alle_change_pH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="8_{B4563AA1-F904-427B-AF4F-96957668340D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{76E28FBB-C54D-48C3-BE39-DFAB772270B9}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{88558B49-1649-4037-AB20-D564493680D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2C17DFF5-11A8-44FA-8A8E-F5D397330A30}"/>
   <bookViews>
-    <workbookView xWindow="-25290" yWindow="675" windowWidth="21600" windowHeight="11280" activeTab="1" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
   </bookViews>
   <sheets>
     <sheet name="pH 9.2" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="17">
   <si>
     <t>Na  [mg/l]</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>fortynding</t>
+  </si>
+  <si>
+    <t>HCO3 [mg/L]</t>
   </si>
 </sst>
 </file>
@@ -573,23 +576,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E6429C-0FFF-4E30-BF3A-6A5B96E649C1}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -627,7 +630,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -653,7 +656,7 @@
         <v>9.11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3.5</v>
       </c>
@@ -679,7 +682,7 @@
         <v>9.19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3.5</v>
       </c>
@@ -708,7 +711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -734,7 +737,7 @@
         <v>9.23</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -760,7 +763,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -786,7 +789,7 @@
         <v>9.24</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -814,7 +817,7 @@
         <v>8.57</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -840,7 +843,7 @@
         <v>9.2799999999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -866,7 +869,7 @@
         <v>8.58</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -892,7 +895,7 @@
         <v>9.32</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -918,16 +921,16 @@
         <v>8.59</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>9</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-9-F</v>
+        <v>M-9.2-8,7-F</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -944,16 +947,16 @@
         <v>9.2899999999999991</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>9</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A14,"-P")</f>
-        <v>M-9.2-9-P</v>
+        <v>M-9.2-8,7-P</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -970,12 +973,15 @@
         <v>8.6300000000000008</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -986,72 +992,39 @@
         <f>CONCATENATE("Bi-M","-9.2-",A18,"-F")</f>
         <v>Bi-M-9.2-0-F</v>
       </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D18" s="2">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="3" t="str">
-        <f t="shared" ref="C19:C23" si="1">CONCATENATE("Bi-M","-9.2-",A19,"-F")</f>
-        <v>Bi-M-9.2-0-F</v>
-      </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" ref="C19:C20" si="1">CONCATENATE("Bi-M","-9.2-",A19,"-F")</f>
+        <v>Bi-M-9.2-6-F</v>
+      </c>
+      <c r="D19" s="2">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>6</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>Bi-M-9.2-6-F</v>
-      </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>6</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Bi-M-9.2-6-F</v>
-      </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>9</v>
-      </c>
-      <c r="B22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Bi-M-9.2-9-F</v>
-      </c>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>9</v>
-      </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Bi-M-9.2-9-F</v>
-      </c>
-      <c r="D23" s="2"/>
+        <v>Bi-M-9.2-8,7-F</v>
+      </c>
+      <c r="D20" s="2">
+        <v>963</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1062,18 +1035,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A17F5B53-D1CD-43A2-82D9-8A2F69E97C05}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1102,7 +1075,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1122,7 +1095,7 @@
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1.25</v>
       </c>
@@ -1142,7 +1115,7 @@
       </c>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1.25</v>
       </c>
@@ -1162,7 +1135,7 @@
       </c>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1182,7 +1155,7 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1202,7 +1175,7 @@
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1222,7 +1195,7 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -1242,7 +1215,7 @@
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -1260,7 +1233,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -1278,7 +1251,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>6</v>
       </c>
@@ -1296,7 +1269,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -1314,7 +1287,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>7</v>
       </c>
@@ -1332,7 +1305,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -1350,12 +1323,15 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -1368,70 +1344,31 @@
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="3" t="str">
-        <f t="shared" ref="C19:C23" si="1">CONCATENATE("Bi-M","-9.2-",A19,"-F")</f>
-        <v>Bi-M-9.2-0-F</v>
+        <f t="shared" ref="C19:C20" si="1">CONCATENATE("Bi-M","-9.2-",A19,"-F")</f>
+        <v>Bi-M-9.2-6-F</v>
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>Bi-M-9.2-6-F</v>
+        <v>Bi-M-9.2-9-F</v>
       </c>
       <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>6</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Bi-M-9.2-6-F</v>
-      </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>9</v>
-      </c>
-      <c r="B22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Bi-M-9.2-9-F</v>
-      </c>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>9</v>
-      </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Bi-M-9.2-9-F</v>
-      </c>
-      <c r="D23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1441,23 +1378,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AF8B36-B0FD-4CC9-B091-FE33E35F5622}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1486,7 +1423,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -1504,7 +1441,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3.5</v>
       </c>
@@ -1522,7 +1459,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3.5</v>
       </c>
@@ -1540,7 +1477,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1558,7 +1495,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1576,7 +1513,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1594,7 +1531,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -1612,7 +1549,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -1630,7 +1567,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7</v>
       </c>
@@ -1648,7 +1585,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -1666,7 +1603,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>8</v>
       </c>
@@ -1684,7 +1621,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>9</v>
       </c>
@@ -1702,7 +1639,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>9</v>
       </c>
@@ -1720,12 +1657,15 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -1738,70 +1678,31 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" s="3" t="str">
-        <f t="shared" ref="C21:C25" si="1">CONCATENATE("Bi-M","-9.2-",A21,"-F")</f>
-        <v>Bi-M-9.2-0-F</v>
+        <f t="shared" ref="C21:C22" si="1">CONCATENATE("Bi-M","-9.2-",A21,"-F")</f>
+        <v>Bi-M-9.2-6-F</v>
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>Bi-M-9.2-6-F</v>
+        <v>Bi-M-9.2-9-F</v>
       </c>
       <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>6</v>
-      </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Bi-M-9.2-6-F</v>
-      </c>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>9</v>
-      </c>
-      <c r="B24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Bi-M-9.2-9-F</v>
-      </c>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>9</v>
-      </c>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Bi-M-9.2-9-F</v>
-      </c>
-      <c r="D25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
SiO2 fra multi pH 10 forsøg
</commit_message>
<xml_diff>
--- a/data/Multi_salt_alle_change_pH.xlsx
+++ b/data/Multi_salt_alle_change_pH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{88558B49-1649-4037-AB20-D564493680D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2C17DFF5-11A8-44FA-8A8E-F5D397330A30}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{88558B49-1649-4037-AB20-D564493680D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{590B408A-5CFB-4969-AF96-C242FD8432A2}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
   </bookViews>
   <sheets>
     <sheet name="pH 9.2" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="18">
   <si>
     <t>Na  [mg/l]</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>HCO3 [mg/L]</t>
+  </si>
+  <si>
+    <t>6.5</t>
   </si>
 </sst>
 </file>
@@ -237,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -262,6 +265,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,21 +582,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E6429C-0FFF-4E30-BF3A-6A5B96E649C1}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -630,7 +634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -656,7 +660,7 @@
         <v>9.11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>3.5</v>
       </c>
@@ -682,7 +686,7 @@
         <v>9.19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3.5</v>
       </c>
@@ -711,7 +715,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -737,7 +741,7 @@
         <v>9.23</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -763,7 +767,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -789,7 +793,7 @@
         <v>9.24</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -817,7 +821,7 @@
         <v>8.57</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -843,7 +847,7 @@
         <v>9.2799999999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -869,7 +873,7 @@
         <v>8.58</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -895,7 +899,7 @@
         <v>9.32</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -921,7 +925,7 @@
         <v>8.59</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>8.6999999999999993</v>
       </c>
@@ -947,7 +951,7 @@
         <v>9.2899999999999991</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>8.6999999999999993</v>
       </c>
@@ -973,7 +977,7 @@
         <v>8.6300000000000008</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>11</v>
       </c>
@@ -981,7 +985,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -996,7 +1000,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>6</v>
       </c>
@@ -1011,7 +1015,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>8.6999999999999993</v>
       </c>
@@ -1037,16 +1041,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A17F5B53-D1CD-43A2-82D9-8A2F69E97C05}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1075,7 +1079,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1095,7 +1099,7 @@
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1.25</v>
       </c>
@@ -1115,7 +1119,7 @@
       </c>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1.25</v>
       </c>
@@ -1135,7 +1139,7 @@
       </c>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1155,7 +1159,7 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1175,7 +1179,7 @@
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1195,7 +1199,7 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -1210,12 +1214,12 @@
       <c r="E8" s="2"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="6">
-        <v>25</v>
+      <c r="H8" s="12">
+        <v>25.9</v>
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -1230,10 +1234,12 @@
       <c r="E9" s="2"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="6"/>
+      <c r="H9" s="6">
+        <v>55.7</v>
+      </c>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -1248,82 +1254,132 @@
       <c r="E10" s="2"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="6">
+        <v>27.3</v>
+      </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>M-9.2-6-F</v>
+        <f t="shared" ref="C11:C12" si="1">CONCATENATE("M","-9.2-",A11,"-F")</f>
+        <v>M-9.2-5,5-F</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
+      <c r="H11" s="6">
+        <v>63.2</v>
+      </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A12,"-P")</f>
-        <v>M-9.2-6-P</v>
+        <v>M-9.2-5,5-P</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="6"/>
+      <c r="H12" s="6">
+        <v>29.6</v>
+      </c>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>M-9.2-7-F</v>
+        <f>CONCATENATE("M","-9.2-",A13,"-F")</f>
+        <v>M-9.2-6-F</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="6"/>
+      <c r="H13" s="6">
+        <v>71</v>
+      </c>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A14,"-P")</f>
-        <v>M-9.2-7-P</v>
+        <v>M-9.2-6-P</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
+      <c r="H14" s="6">
+        <v>30.7</v>
+      </c>
       <c r="I14" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3" t="str">
+        <f>CONCATENATE("M","-9.2-",A15,"-F")</f>
+        <v>M-9.2-6.5-F</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6">
+        <v>78.5</v>
+      </c>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="3" t="str">
+        <f>CONCATENATE("M","-9.2-",A16,"-P")</f>
+        <v>M-9.2-6.5-P</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6">
+        <v>32.4</v>
+      </c>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>11</v>
       </c>
@@ -1331,7 +1387,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -1344,7 +1400,7 @@
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>6</v>
       </c>
@@ -1352,12 +1408,12 @@
         <v>2</v>
       </c>
       <c r="C19" s="3" t="str">
-        <f t="shared" ref="C19:C20" si="1">CONCATENATE("Bi-M","-9.2-",A19,"-F")</f>
+        <f t="shared" ref="C19:C20" si="2">CONCATENATE("Bi-M","-9.2-",A19,"-F")</f>
         <v>Bi-M-9.2-6-F</v>
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>9</v>
       </c>
@@ -1365,7 +1421,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Bi-M-9.2-9-F</v>
       </c>
       <c r="D20" s="2"/>
@@ -1384,17 +1440,17 @@
       <selection activeCell="A24" sqref="A24:D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1423,7 +1479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -1441,7 +1497,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3.5</v>
       </c>
@@ -1459,7 +1515,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3.5</v>
       </c>
@@ -1477,7 +1533,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1495,7 +1551,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1513,7 +1569,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1531,7 +1587,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -1549,7 +1605,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -1567,7 +1623,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>7</v>
       </c>
@@ -1585,7 +1641,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -1603,7 +1659,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>8</v>
       </c>
@@ -1621,7 +1677,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>9</v>
       </c>
@@ -1639,7 +1695,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>9</v>
       </c>
@@ -1657,7 +1713,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>11</v>
       </c>
@@ -1665,7 +1721,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -1678,7 +1734,7 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>6</v>
       </c>
@@ -1691,7 +1747,7 @@
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
data behandling for 10.5
</commit_message>
<xml_diff>
--- a/data/Multi_salt_alle_change_pH.xlsx
+++ b/data/Multi_salt_alle_change_pH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{88558B49-1649-4037-AB20-D564493680D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{590B408A-5CFB-4969-AF96-C242FD8432A2}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{88558B49-1649-4037-AB20-D564493680D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AE488DC6-71FD-4071-A8F4-2BFE2588611C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
   </bookViews>
   <sheets>
     <sheet name="pH 9.2" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="18">
   <si>
     <t>Na  [mg/l]</t>
   </si>
@@ -1041,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A17F5B53-D1CD-43A2-82D9-8A2F69E97C05}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1087,7 +1087,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="str">
-        <f t="shared" ref="C2:C13" si="0">CONCATENATE("M","-9.2-",A2,"-F")</f>
+        <f t="shared" ref="C2:C9" si="0">CONCATENATE("M","-9.2-",A2,"-F")</f>
         <v>M-9.2-0-F</v>
       </c>
       <c r="D2" s="2"/>
@@ -1267,7 +1267,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="3" t="str">
-        <f t="shared" ref="C11:C12" si="1">CONCATENATE("M","-9.2-",A11,"-F")</f>
+        <f t="shared" ref="C11" si="1">CONCATENATE("M","-9.2-",A11,"-F")</f>
         <v>M-9.2-5,5-F</v>
       </c>
       <c r="D11" s="2"/>
@@ -1436,13 +1436,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AF8B36-B0FD-4CC9-B091-FE33E35F5622}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -1494,226 +1496,292 @@
       <c r="E4" s="2"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
+      <c r="H4" s="6">
+        <v>40.1</v>
+      </c>
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-3,5-F</v>
+        <v>M-9.2-2,5-F</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
+      <c r="H5" s="6">
+        <v>49.4</v>
+      </c>
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A6,"-P")</f>
-        <v>M-9.2-3,5-P</v>
+        <v>M-9.2-2,5-P</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
+      <c r="H6" s="6">
+        <v>16.899999999999999</v>
+      </c>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-5-F</v>
+        <v>M-9.2-4-F</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
+      <c r="H7" s="6">
+        <v>52.2</v>
+      </c>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A8,"-P")</f>
-        <v>M-9.2-5-P</v>
+        <v>M-9.2-4-P</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
+      <c r="H8" s="6">
+        <v>18.7</v>
+      </c>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-6-F</v>
+        <v>M-9.2-5-F</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="6"/>
+      <c r="H9" s="6">
+        <v>61.1</v>
+      </c>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A10,"-P")</f>
-        <v>M-9.2-6-P</v>
+        <v>M-9.2-5-P</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="6">
+        <v>19.899999999999999</v>
+      </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-7-F</v>
+        <v>M-9.2-6-F</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
+      <c r="H11" s="6">
+        <v>67.2</v>
+      </c>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A12,"-P")</f>
-        <v>M-9.2-7-P</v>
+        <v>M-9.2-6-P</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="6"/>
+      <c r="H12" s="6">
+        <v>21.5</v>
+      </c>
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-8-F</v>
+        <v>M-9.2-7-F</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="6"/>
+      <c r="H13" s="6">
+        <v>81.400000000000006</v>
+      </c>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A14,"-P")</f>
-        <v>M-9.2-8-P</v>
+        <v>M-9.2-7-P</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
+      <c r="H14" s="6">
+        <v>24</v>
+      </c>
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-9-F</v>
+        <v>M-9.2-8-F</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
+      <c r="H15" s="6">
+        <v>98</v>
+      </c>
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A16,"-P")</f>
-        <v>M-9.2-9-P</v>
+        <v>M-9.2-8-P</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
+      <c r="H16" s="6">
+        <v>26.8</v>
+      </c>
       <c r="I16" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>8.17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3" t="str">
+        <f t="shared" ref="C17" si="1">CONCATENATE("M","-9.2-",A17,"-F")</f>
+        <v>M-9.2-8,17-F</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="6">
+        <v>97.7</v>
+      </c>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>8.17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="3" t="str">
+        <f>CONCATENATE("M","-9.2-",A18,"-P")</f>
+        <v>M-9.2-8,17-P</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="6">
+        <v>28</v>
+      </c>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>11</v>
       </c>
@@ -1721,7 +1789,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -1734,7 +1802,7 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>6</v>
       </c>
@@ -1742,12 +1810,12 @@
         <v>2</v>
       </c>
       <c r="C21" s="3" t="str">
-        <f t="shared" ref="C21:C22" si="1">CONCATENATE("Bi-M","-9.2-",A21,"-F")</f>
+        <f t="shared" ref="C21:C22" si="2">CONCATENATE("Bi-M","-9.2-",A21,"-F")</f>
         <v>Bi-M-9.2-6-F</v>
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>9</v>
       </c>
@@ -1755,7 +1823,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Bi-M-9.2-9-F</v>
       </c>
       <c r="D22" s="2"/>

</xml_diff>

<commit_message>
Tilføjet pH 10.5 samt bicarbonat
</commit_message>
<xml_diff>
--- a/data/Multi_salt_alle_change_pH.xlsx
+++ b/data/Multi_salt_alle_change_pH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{88558B49-1649-4037-AB20-D564493680D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AE488DC6-71FD-4071-A8F4-2BFE2588611C}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="8_{88558B49-1649-4037-AB20-D564493680D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B2FDAA01-430B-4191-9D92-288698EF9EE4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
+    <workbookView xWindow="5025" yWindow="1575" windowWidth="21600" windowHeight="11280" activeTab="1" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
   </bookViews>
   <sheets>
     <sheet name="pH 9.2" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="17">
   <si>
     <t>Na  [mg/l]</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t xml:space="preserve">Bicarbonate </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC analyse </t>
   </si>
   <si>
     <t>con</t>
@@ -583,7 +580,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,13 +622,13 @@
         <v>7</v>
       </c>
       <c r="J1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>14</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -982,7 +979,7 @@
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1041,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A17F5B53-D1CD-43A2-82D9-8A2F69E97C05}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1341,7 +1338,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
@@ -1361,7 +1358,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -1384,7 +1381,7 @@
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1398,33 +1395,39 @@
         <f>CONCATENATE("Bi-M","-9.2-",A18,"-F")</f>
         <v>Bi-M-9.2-0-F</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" s="2">
+        <v>373</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="3" t="str">
         <f t="shared" ref="C19:C20" si="2">CONCATENATE("Bi-M","-9.2-",A19,"-F")</f>
-        <v>Bi-M-9.2-6-F</v>
-      </c>
-      <c r="D19" s="2"/>
+        <v>Bi-M-9.2-4-F</v>
+      </c>
+      <c r="D19" s="2">
+        <v>595</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>9</v>
+      <c r="A20" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>Bi-M-9.2-9-F</v>
-      </c>
-      <c r="D20" s="2"/>
+        <v>Bi-M-9.2-6.5-F</v>
+      </c>
+      <c r="D20" s="2">
+        <v>998</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1434,10 +1437,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AF8B36-B0FD-4CC9-B091-FE33E35F5622}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1448,385 +1451,380 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="str">
+        <f t="shared" ref="C2:C13" si="0">CONCATENATE("M","-9.2-",A2,"-F")</f>
+        <v>M-9.2-0-F</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6">
+        <v>40.1</v>
+      </c>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
+      <c r="A3" s="1">
+        <v>2.5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>7</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>M-9.2-2,5-F</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6">
+        <v>49.4</v>
+      </c>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="str">
-        <f t="shared" ref="C4:C15" si="0">CONCATENATE("M","-9.2-",A4,"-F")</f>
-        <v>M-9.2-0-F</v>
+        <f>CONCATENATE("M","-9.2-",A4,"-P")</f>
+        <v>M-9.2-2,5-P</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="6">
-        <v>40.1</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-2,5-F</v>
+        <v>M-9.2-4-F</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="6">
-        <v>49.4</v>
+        <v>52.2</v>
       </c>
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A6,"-P")</f>
-        <v>M-9.2-2,5-P</v>
+        <v>M-9.2-4-P</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="6">
-        <v>16.899999999999999</v>
+        <v>18.7</v>
       </c>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-4-F</v>
+        <v>M-9.2-5-F</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="6">
-        <v>52.2</v>
+        <v>61.1</v>
       </c>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A8,"-P")</f>
-        <v>M-9.2-4-P</v>
+        <v>M-9.2-5-P</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="6">
-        <v>18.7</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-5-F</v>
+        <v>M-9.2-6-F</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="6">
-        <v>61.1</v>
+        <v>67.2</v>
       </c>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A10,"-P")</f>
-        <v>M-9.2-5-P</v>
+        <v>M-9.2-6-P</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="6">
-        <v>19.899999999999999</v>
+        <v>21.5</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-6-F</v>
+        <v>M-9.2-7-F</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="6">
-        <v>67.2</v>
+        <v>81.400000000000006</v>
       </c>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A12,"-P")</f>
-        <v>M-9.2-6-P</v>
+        <v>M-9.2-7-P</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="6">
-        <v>21.5</v>
+        <v>24</v>
       </c>
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>M-9.2-7-F</v>
+        <v>M-9.2-8-F</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="6">
-        <v>81.400000000000006</v>
+        <v>98</v>
       </c>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A14,"-P")</f>
-        <v>M-9.2-7-P</v>
+        <v>M-9.2-8-P</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="6">
-        <v>24</v>
+        <v>26.8</v>
       </c>
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>8</v>
+        <v>8.17</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>M-9.2-8-F</v>
+        <f t="shared" ref="C15" si="1">CONCATENATE("M","-9.2-",A15,"-F")</f>
+        <v>M-9.2-8,17-F</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="6">
-        <v>98</v>
+        <v>97.7</v>
       </c>
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>8</v>
+        <v>8.17</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="3" t="str">
         <f>CONCATENATE("M","-9.2-",A16,"-P")</f>
-        <v>M-9.2-8-P</v>
+        <v>M-9.2-8,17-P</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="6">
-        <v>26.8</v>
+        <v>28</v>
       </c>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>8.17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="3" t="str">
-        <f t="shared" ref="C17" si="1">CONCATENATE("M","-9.2-",A17,"-F")</f>
-        <v>M-9.2-8,17-F</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="6">
-        <v>97.7</v>
-      </c>
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>8.17</v>
+        <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18" s="3" t="str">
-        <f>CONCATENATE("M","-9.2-",A18,"-P")</f>
-        <v>M-9.2-8,17-P</v>
+        <f>CONCATENATE("Bi-M","-9.2-",A18,"-F")</f>
+        <v>Bi-M-9.2-0-F</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="6">
-        <v>28</v>
-      </c>
-      <c r="I18" s="6"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="3" t="str">
+        <f t="shared" ref="C19:C20" si="2">CONCATENATE("Bi-M","-9.2-",A19,"-F")</f>
+        <v>Bi-M-9.2-6-F</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="3" t="str">
-        <f>CONCATENATE("Bi-M","-9.2-",A20,"-F")</f>
-        <v>Bi-M-9.2-0-F</v>
-      </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>6</v>
-      </c>
-      <c r="B21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="3" t="str">
-        <f t="shared" ref="C21:C22" si="2">CONCATENATE("Bi-M","-9.2-",A21,"-F")</f>
-        <v>Bi-M-9.2-6-F</v>
-      </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>9</v>
-      </c>
-      <c r="B22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Bi-M-9.2-9-F</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
data behandling med DIT-M mm
</commit_message>
<xml_diff>
--- a/data/Multi_salt_alle_change_pH.xlsx
+++ b/data/Multi_salt_alle_change_pH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="8_{88558B49-1649-4037-AB20-D564493680D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{739AEC35-9E99-41FD-A0EC-2384C54FB344}"/>
+  <xr:revisionPtr revIDLastSave="220" documentId="8_{88558B49-1649-4037-AB20-D564493680D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8E6F78C8-5086-4148-9E1C-3D20D18228BF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
+    <workbookView xWindow="1110" yWindow="285" windowWidth="27000" windowHeight="14235" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
   </bookViews>
   <sheets>
     <sheet name="pH 9.2" sheetId="1" r:id="rId1"/>
@@ -35,42 +35,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Steffen Lykke Christensen</author>
-  </authors>
-  <commentList>
-    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{326DB34D-FEAC-4F14-AE49-3242A1440A67}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Steffen Lykke Christensen:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-repetition af 6p</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="18">
   <si>
     <t>Na  [mg/l]</t>
   </si>
@@ -123,14 +89,14 @@
     <t>6.5</t>
   </si>
   <si>
-    <t>cl</t>
+    <t>DIT-M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,19 +111,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -240,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -269,6 +222,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,24 +536,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E6429C-0FFF-4E30-BF3A-6A5B96E649C1}">
-  <dimension ref="A1:S20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E6429C-0FFF-4E30-BF3A-6A5B96E649C1}">
+  <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -628,37 +582,26 @@
         <v>7</v>
       </c>
       <c r="J1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="R1" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O1" s="11"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -677,23 +620,25 @@
         <v>40.4</v>
       </c>
       <c r="I2" s="6">
-        <v>19.600000000000001</v>
+        <v>9.4</v>
       </c>
       <c r="J2">
+        <v>25</v>
+      </c>
+      <c r="K2">
+        <f>I2*J2</f>
+        <v>235</v>
+      </c>
+      <c r="L2">
         <v>1339</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>9.11</v>
       </c>
-      <c r="L2">
-        <v>10</v>
-      </c>
-      <c r="M2">
-        <f>I2*L2</f>
-        <v>196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O2" s="3"/>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3.5</v>
       </c>
@@ -712,43 +657,26 @@
         <v>42.9</v>
       </c>
       <c r="I3" s="6">
-        <v>4.8</v>
+        <v>6.8</v>
       </c>
       <c r="J3">
+        <v>25</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K14" si="1">I3*J3</f>
+        <v>170</v>
+      </c>
+      <c r="L3">
         <v>1527</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>9.19</v>
       </c>
-      <c r="L3">
-        <v>100</v>
-      </c>
-      <c r="M3" s="3">
-        <f t="shared" ref="M3:M14" si="1">I3*L3</f>
-        <v>480</v>
-      </c>
-      <c r="N3">
-        <v>6.7</v>
-      </c>
-      <c r="O3">
-        <v>50</v>
-      </c>
-      <c r="P3" s="3">
-        <f>N3*O3</f>
-        <v>335</v>
-      </c>
-      <c r="Q3">
-        <v>10.4</v>
-      </c>
-      <c r="R3">
-        <v>25</v>
-      </c>
-      <c r="S3" s="3">
-        <f>Q3*R3</f>
-        <v>260</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="U3" s="3"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3.5</v>
       </c>
@@ -766,16 +694,23 @@
       <c r="H4" s="6">
         <v>33.799999999999997</v>
       </c>
-      <c r="I4" s="6"/>
+      <c r="I4" s="6">
+        <v>9</v>
+      </c>
       <c r="J4">
+        <v>25</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>225</v>
+      </c>
+      <c r="L4">
         <v>813</v>
       </c>
-      <c r="M4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O4" s="3"/>
+      <c r="R4" s="3"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -794,23 +729,25 @@
         <v>42.2</v>
       </c>
       <c r="I5" s="6">
-        <v>4.4000000000000004</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="J5">
+        <v>25</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>242.49999999999997</v>
+      </c>
+      <c r="L5">
         <v>1708</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>9.23</v>
       </c>
-      <c r="L5">
-        <v>100</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="1"/>
-        <v>440.00000000000006</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O5" s="3"/>
+      <c r="R5" s="3"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -828,19 +765,26 @@
       <c r="H6" s="6">
         <v>35.5</v>
       </c>
-      <c r="I6" s="6"/>
+      <c r="I6" s="6">
+        <v>10.199999999999999</v>
+      </c>
       <c r="J6">
+        <v>25</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>254.99999999999997</v>
+      </c>
+      <c r="L6">
         <v>882</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>8.56</v>
       </c>
-      <c r="M6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O6" s="3"/>
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -858,19 +802,26 @@
       <c r="H7" s="6">
         <v>45.3</v>
       </c>
-      <c r="I7" s="6"/>
+      <c r="I7" s="6">
+        <v>9.4</v>
+      </c>
       <c r="J7">
+        <v>25</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>235</v>
+      </c>
+      <c r="L7">
         <v>1856</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>9.24</v>
       </c>
-      <c r="M7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O7" s="3"/>
+      <c r="R7" s="3"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -889,20 +840,25 @@
         <v>41.3</v>
       </c>
       <c r="I8" s="6">
-        <v>36.5</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="J8">
+        <v>25</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>229.99999999999997</v>
+      </c>
+      <c r="L8">
         <v>945</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>8.57</v>
       </c>
-      <c r="M8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O8" s="3"/>
+      <c r="R8" s="3"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -920,19 +876,26 @@
       <c r="H9" s="6">
         <v>48.4</v>
       </c>
-      <c r="I9" s="6"/>
+      <c r="I9" s="6">
+        <v>9.1999999999999993</v>
+      </c>
       <c r="J9">
+        <v>25</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>229.99999999999997</v>
+      </c>
+      <c r="L9">
         <v>2050</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>9.2799999999999994</v>
       </c>
-      <c r="M9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O9" s="3"/>
+      <c r="R9" s="3"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -952,17 +915,22 @@
       </c>
       <c r="I10" s="6"/>
       <c r="J10">
-        <v>1027</v>
+        <v>25</v>
       </c>
       <c r="K10">
-        <v>8.58</v>
-      </c>
-      <c r="M10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <v>1027</v>
+      </c>
+      <c r="M10">
+        <v>8.58</v>
+      </c>
+      <c r="O10" s="3"/>
+      <c r="R10" s="3"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -980,19 +948,26 @@
       <c r="H11" s="6">
         <v>50.2</v>
       </c>
-      <c r="I11" s="6"/>
+      <c r="I11" s="6">
+        <v>7.5</v>
+      </c>
       <c r="J11">
+        <v>25</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>187.5</v>
+      </c>
+      <c r="L11">
         <v>2350</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>9.32</v>
       </c>
-      <c r="M11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O11" s="3"/>
+      <c r="R11" s="3"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -1012,17 +987,22 @@
       </c>
       <c r="I12" s="6"/>
       <c r="J12">
-        <v>1130</v>
+        <v>25</v>
       </c>
       <c r="K12">
-        <v>8.59</v>
-      </c>
-      <c r="M12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="L12">
+        <v>1130</v>
+      </c>
+      <c r="M12">
+        <v>8.59</v>
+      </c>
+      <c r="O12" s="3"/>
+      <c r="R12" s="3"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8.6999999999999993</v>
       </c>
@@ -1040,19 +1020,26 @@
       <c r="H13" s="6">
         <v>55.4</v>
       </c>
-      <c r="I13" s="6"/>
+      <c r="I13" s="6">
+        <v>7.1</v>
+      </c>
       <c r="J13">
+        <v>25</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>177.5</v>
+      </c>
+      <c r="L13">
         <v>2710</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <v>9.2899999999999991</v>
       </c>
-      <c r="M13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O13" s="3"/>
+      <c r="R13" s="3"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>8.6999999999999993</v>
       </c>
@@ -1070,19 +1057,30 @@
       <c r="H14" s="6">
         <v>40.200000000000003</v>
       </c>
-      <c r="I14" s="6"/>
+      <c r="I14" s="6">
+        <v>10</v>
+      </c>
       <c r="J14">
+        <v>25</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="L14">
         <v>1133</v>
       </c>
-      <c r="K14">
+      <c r="M14">
         <v>8.6300000000000008</v>
       </c>
-      <c r="M14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="O14" s="3"/>
+      <c r="R14" s="3"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M15" s="14"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>11</v>
       </c>
@@ -1090,7 +1088,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -1105,7 +1103,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>6</v>
       </c>
@@ -1120,7 +1118,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>8.6999999999999993</v>
       </c>
@@ -1138,7 +1136,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1150,12 +1147,12 @@
       <selection activeCell="K17" sqref="K1:K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1185,7 +1182,7 @@
       </c>
       <c r="K1" s="13"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1205,7 +1202,7 @@
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1.25</v>
       </c>
@@ -1225,7 +1222,7 @@
       </c>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1.25</v>
       </c>
@@ -1245,7 +1242,7 @@
       </c>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1265,7 +1262,7 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1285,7 +1282,7 @@
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1305,7 +1302,7 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -1325,7 +1322,7 @@
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -1345,7 +1342,7 @@
       </c>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -1365,7 +1362,7 @@
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>5.5</v>
       </c>
@@ -1385,7 +1382,7 @@
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>5.5</v>
       </c>
@@ -1405,7 +1402,7 @@
       </c>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>6</v>
       </c>
@@ -1425,7 +1422,7 @@
       </c>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>6</v>
       </c>
@@ -1445,7 +1442,7 @@
       </c>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1465,7 +1462,7 @@
       </c>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1485,7 +1482,7 @@
       </c>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>11</v>
       </c>
@@ -1493,7 +1490,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -1508,7 +1505,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>4</v>
       </c>
@@ -1523,7 +1520,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -1549,17 +1546,17 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="K1:L19"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1587,9 +1584,14 @@
       <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="13"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1609,7 +1611,7 @@
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2.5</v>
       </c>
@@ -1629,7 +1631,7 @@
       </c>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2.5</v>
       </c>
@@ -1649,7 +1651,7 @@
       </c>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1669,7 +1671,7 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1689,7 +1691,7 @@
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1709,7 +1711,7 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1729,7 +1731,7 @@
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1749,7 +1751,7 @@
       </c>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -1769,7 +1771,7 @@
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -1789,7 +1791,7 @@
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7</v>
       </c>
@@ -1809,7 +1811,7 @@
       </c>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -1829,7 +1831,7 @@
       </c>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>8</v>
       </c>
@@ -1849,7 +1851,7 @@
       </c>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>8.17</v>
       </c>
@@ -1867,9 +1869,18 @@
       <c r="H15" s="6">
         <v>97.7</v>
       </c>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I15" s="6">
+        <v>7.2</v>
+      </c>
+      <c r="J15">
+        <v>25</v>
+      </c>
+      <c r="K15">
+        <f>I15*J15</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>8.17</v>
       </c>
@@ -1889,7 +1900,7 @@
       </c>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>11</v>
       </c>
@@ -1897,7 +1908,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -1910,7 +1921,7 @@
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>6</v>
       </c>
@@ -1923,7 +1934,7 @@
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
plot af ny IC data pH 9.2
</commit_message>
<xml_diff>
--- a/data/Multi_salt_alle_change_pH.xlsx
+++ b/data/Multi_salt_alle_change_pH.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/992765_grundfos_com/Documents/Code/Speciale/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="8_{88558B49-1649-4037-AB20-D564493680D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8E6F78C8-5086-4148-9E1C-3D20D18228BF}"/>
+  <xr:revisionPtr revIDLastSave="233" documentId="8_{88558B49-1649-4037-AB20-D564493680D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FF513328-4039-460C-94DC-810702A4C828}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="285" windowWidth="27000" windowHeight="14235" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
   </bookViews>
   <sheets>
     <sheet name="pH 9.2" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,160 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Susan Ottesen</author>
+  </authors>
+  <commentList>
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{0B07A783-14EA-4980-99DC-EA6766E956C9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Susan Ottesen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Kan ikke aflæses</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{8453D227-2321-40D5-80C2-C335551FC56B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Susan Ottesen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Kan ikke aflæses</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{1E62E7F7-8819-4527-85F4-4762DDA21658}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Susan Ottesen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Kan ikke aflæses</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{34A21BCE-3182-4D3F-A43C-0FB73D9DB5E6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Susan Ottesen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Kan ikke aflæses</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{096893E0-D92E-4C43-A184-9CB87DEB516C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Susan Ottesen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Kan ikke aflæses</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{ED0EE5E6-4C79-4539-ABCD-7305AF6F9A3F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Susan Ottesen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Kan ikke aflæses</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -96,7 +250,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +265,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -536,11 +703,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E6429C-0FFF-4E30-BF3A-6A5B96E649C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E6429C-0FFF-4E30-BF3A-6A5B96E649C1}">
   <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,10 +779,18 @@
         <f t="shared" ref="C2:C13" si="0">CONCATENATE("M","-9.2-",A2,"-F")</f>
         <v>M-9.2-0-F</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="D2" s="2">
+        <v>301</v>
+      </c>
+      <c r="E2" s="2">
+        <v>137</v>
+      </c>
+      <c r="F2" s="2">
+        <v>71</v>
+      </c>
+      <c r="G2" s="2">
+        <v>7.9</v>
+      </c>
       <c r="H2" s="6">
         <v>40.4</v>
       </c>
@@ -649,10 +824,18 @@
         <f t="shared" si="0"/>
         <v>M-9.2-3,5-F</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="D3" s="2">
+        <v>344</v>
+      </c>
+      <c r="E3" s="2">
+        <v>131</v>
+      </c>
+      <c r="F3" s="2">
+        <v>98</v>
+      </c>
+      <c r="G3" s="2">
+        <v>24</v>
+      </c>
       <c r="H3" s="6">
         <v>42.9</v>
       </c>
@@ -687,10 +870,16 @@
         <f>CONCATENATE("M","-9.2-",A4,"-P")</f>
         <v>M-9.2-3,5-P</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="D4" s="2">
+        <v>173</v>
+      </c>
+      <c r="E4" s="2">
+        <v>132</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2">
+        <v>5.2</v>
+      </c>
       <c r="H4" s="6">
         <v>33.799999999999997</v>
       </c>
@@ -721,10 +910,18 @@
         <f t="shared" si="0"/>
         <v>M-9.2-5-F</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="D5" s="2">
+        <v>390</v>
+      </c>
+      <c r="E5" s="2">
+        <v>132</v>
+      </c>
+      <c r="F5" s="2">
+        <v>126</v>
+      </c>
+      <c r="G5" s="2">
+        <v>29</v>
+      </c>
       <c r="H5" s="6">
         <v>42.2</v>
       </c>
@@ -758,10 +955,16 @@
         <f>CONCATENATE("M","-9.2-",A6,"-P")</f>
         <v>M-9.2-5-P</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="D6" s="2">
+        <v>194</v>
+      </c>
+      <c r="E6" s="2">
+        <v>136</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2">
+        <v>5.8</v>
+      </c>
       <c r="H6" s="6">
         <v>35.5</v>
       </c>
@@ -795,10 +998,18 @@
         <f t="shared" si="0"/>
         <v>M-9.2-6-F</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="D7" s="2">
+        <v>425</v>
+      </c>
+      <c r="E7" s="2">
+        <v>131</v>
+      </c>
+      <c r="F7" s="2">
+        <v>150</v>
+      </c>
+      <c r="G7" s="2">
+        <v>34</v>
+      </c>
       <c r="H7" s="6">
         <v>45.3</v>
       </c>
@@ -832,10 +1043,16 @@
         <f>CONCATENATE("M","-9.2-",A8,"-P")</f>
         <v>M-9.2-6-P</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="D8" s="2">
+        <v>200</v>
+      </c>
+      <c r="E8" s="2">
+        <v>134</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2">
+        <v>5.8</v>
+      </c>
       <c r="H8" s="6">
         <v>41.3</v>
       </c>
@@ -869,10 +1086,18 @@
         <f t="shared" si="0"/>
         <v>M-9.2-7-F</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="D9" s="2">
+        <v>473</v>
+      </c>
+      <c r="E9" s="2">
+        <v>128</v>
+      </c>
+      <c r="F9" s="2">
+        <v>182</v>
+      </c>
+      <c r="G9" s="2">
+        <v>40</v>
+      </c>
       <c r="H9" s="6">
         <v>48.4</v>
       </c>
@@ -906,10 +1131,16 @@
         <f>CONCATENATE("M","-9.2-",A10,"-P")</f>
         <v>M-9.2-7-P</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="D10" s="2">
+        <v>222</v>
+      </c>
+      <c r="E10" s="2">
+        <v>137</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2">
+        <v>6.5</v>
+      </c>
       <c r="H10" s="6">
         <v>37.299999999999997</v>
       </c>
@@ -941,10 +1172,18 @@
         <f t="shared" si="0"/>
         <v>M-9.2-8-F</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="D11" s="2">
+        <v>520</v>
+      </c>
+      <c r="E11" s="2">
+        <v>120</v>
+      </c>
+      <c r="F11" s="2">
+        <v>215</v>
+      </c>
+      <c r="G11" s="2">
+        <v>46</v>
+      </c>
       <c r="H11" s="6">
         <v>50.2</v>
       </c>
@@ -978,10 +1217,16 @@
         <f>CONCATENATE("M","-9.2-",A12,"-P")</f>
         <v>M-9.2-8-P</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="D12" s="2">
+        <v>250</v>
+      </c>
+      <c r="E12" s="2">
+        <v>136</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2">
+        <v>7.2</v>
+      </c>
       <c r="H12" s="6">
         <v>38.299999999999997</v>
       </c>
@@ -1013,10 +1258,18 @@
         <f t="shared" si="0"/>
         <v>M-9.2-8,7-F</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="D13" s="2">
+        <v>625</v>
+      </c>
+      <c r="E13" s="2">
+        <v>125</v>
+      </c>
+      <c r="F13" s="2">
+        <v>311</v>
+      </c>
+      <c r="G13" s="2">
+        <v>30</v>
+      </c>
       <c r="H13" s="6">
         <v>55.4</v>
       </c>
@@ -1050,10 +1303,16 @@
         <f>CONCATENATE("M","-9.2-",A14,"-P")</f>
         <v>M-9.2-8,7-P</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="D14" s="2">
+        <v>256</v>
+      </c>
+      <c r="E14" s="2">
+        <v>137</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2">
+        <v>7.2</v>
+      </c>
       <c r="H14" s="6">
         <v>40.200000000000003</v>
       </c>
@@ -1136,6 +1395,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
flere ting efter fuckup
</commit_message>
<xml_diff>
--- a/data/Multi_salt_alle_change_pH.xlsx
+++ b/data/Multi_salt_alle_change_pH.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/992765_grundfos_com/Documents/Code/Speciale/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="233" documentId="8_{88558B49-1649-4037-AB20-D564493680D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FF513328-4039-460C-94DC-810702A4C828}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
   </bookViews>
   <sheets>
     <sheet name="pH 9.2" sheetId="1" r:id="rId1"/>
@@ -706,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E6429C-0FFF-4E30-BF3A-6A5B96E649C1}">
   <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>

</xml_diff>